<commit_message>
Added New Pi Holder
</commit_message>
<xml_diff>
--- a/Electronics Design/Raspberry Pi Interface Board/Default Configuration/Outputs/BOM/BOM_PartType-Raspberry Pi Interface Board.xlsx
+++ b/Electronics Design/Raspberry Pi Interface Board/Default Configuration/Outputs/BOM/BOM_PartType-Raspberry Pi Interface Board.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21750" windowHeight="13185"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19725" windowHeight="8085"/>
   </bookViews>
   <sheets>
     <sheet name="BOM_PartType-Raspberry Pi Inter" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="79">
   <si>
     <t>Designator</t>
   </si>
@@ -42,7 +42,7 @@
     <t>Description</t>
   </si>
   <si>
-    <t>C1, C4, C6</t>
+    <t>C1, C4, C6, C7, C8</t>
   </si>
   <si>
     <t>311-1140-1-ND</t>
@@ -60,7 +60,7 @@
     <t>Capacitor</t>
   </si>
   <si>
-    <t>C2</t>
+    <t>C2, C5</t>
   </si>
   <si>
     <t>1276-6454-1-ND</t>
@@ -75,9 +75,6 @@
     <t>1276-CL21A226MAYNNNECT-ND</t>
   </si>
   <si>
-    <t>C5</t>
-  </si>
-  <si>
     <t>D1</t>
   </si>
   <si>
@@ -93,6 +90,12 @@
     <t>D2</t>
   </si>
   <si>
+    <t>F6271CT-ND</t>
+  </si>
+  <si>
+    <t>Littelfuse Inc.</t>
+  </si>
+  <si>
     <t>TVS Diode</t>
   </si>
   <si>
@@ -111,7 +114,7 @@
     <t>2 Pin Jumper</t>
   </si>
   <si>
-    <t>P1</t>
+    <t>P1, P3</t>
   </si>
   <si>
     <t>732-10955-ND</t>
@@ -177,6 +180,24 @@
     <t>311-10KARCT-ND</t>
   </si>
   <si>
+    <t>R8</t>
+  </si>
+  <si>
+    <t>P1MDACT-ND</t>
+  </si>
+  <si>
+    <t>Panasonic Electronic Components</t>
+  </si>
+  <si>
+    <t>R9, R10</t>
+  </si>
+  <si>
+    <t>541-4129-1-ND</t>
+  </si>
+  <si>
+    <t>Vishay Dale</t>
+  </si>
+  <si>
     <t>RPI1</t>
   </si>
   <si>
@@ -226,12 +247,21 @@
   </si>
   <si>
     <t>Temperature Sensor Digital, Local -40°C ~ 125°C 12 b 8-MSOP</t>
+  </si>
+  <si>
+    <t>U5</t>
+  </si>
+  <si>
+    <t>150-MCP96L01T-E/MXCT-ND</t>
+  </si>
+  <si>
+    <t>Thermocouple EMF to Temperature Converter,  ±1.5°C Maximum Accuracy</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -358,9 +388,9 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -393,9 +423,9 @@
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -575,7 +605,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -618,7 +648,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>8</v>
@@ -641,7 +671,7 @@
         <v>13</v>
       </c>
       <c r="B3" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>14</v>
@@ -690,191 +720,191 @@
         <v>1</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B6" s="3">
         <v>1</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>11</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B7" s="3">
         <v>1</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B8" s="3">
         <v>1</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B9" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="B10" s="3">
         <v>1</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B11" s="3">
         <v>1</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>9</v>
+        <v>40</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="B12" s="3">
         <v>1</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>38</v>
+        <v>9</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>39</v>
+        <v>10</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>11</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="B13" s="3">
         <v>1</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>9</v>
@@ -886,18 +916,18 @@
         <v>11</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B14" s="3">
         <v>1</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>9</v>
@@ -909,18 +939,18 @@
         <v>11</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B15" s="3">
         <v>1</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>9</v>
@@ -932,18 +962,18 @@
         <v>11</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B16" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>9</v>
@@ -955,149 +985,195 @@
         <v>11</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B17" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>10</v>
+        <v>55</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>11</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B18" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>9</v>
+        <v>58</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="B19" s="3">
         <v>1</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>55</v>
+        <v>9</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>56</v>
+        <v>9</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B20" s="3">
         <v>1</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>11</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B21" s="3">
         <v>1</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>11</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B22" s="3">
         <v>1</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>11</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>68</v>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B23" s="3">
+        <v>1</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B24" s="3">
+        <v>1</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>